<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-11-11.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-11-11.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-11-11.xlsx
@@ -1034,6 +1034,9 @@
       <c r="C71" t="str">
         <v>419_松虫草红_scabiosa watermelon_undefined_1bunch</v>
       </c>
+      <c r="F71" t="str">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -1095,7 +1098,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>06101235122013.510581231812955512101035801010568555585166555553823010101015159131055301015510105101015910200</v>
+        <v>06101235122013.510581231812955512101035801010568555585166555553823010101015159131055301015510105101015910202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>